<commit_message>
considerable refactoring and mcm implementation by William fully incorporated
</commit_message>
<xml_diff>
--- a/scales.xlsx
+++ b/scales.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lars/Documents/_Senior Year/mpi/disease control/git/disease-control/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lars/Documents/_Senior Year/mpi/disease control/git-online/disease-control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E21357-11CD-064B-BDCD-554580B72F9E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC52869-4817-F14A-967F-4E4502F4CEF6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="460" windowWidth="23360" windowHeight="17540" xr2:uid="{5FFE7DB9-8542-6846-B116-E5841706403B}"/>
+    <workbookView xWindow="960" yWindow="480" windowWidth="23360" windowHeight="17540" xr2:uid="{5FFE7DB9-8542-6846-B116-E5841706403B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="current" sheetId="2" r:id="rId1"/>
+    <sheet name="old" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
   <si>
     <t>Scales of heuristic intensities to match stochastic optimal control interventions over time window [0.0, 10.0]</t>
   </si>
@@ -106,6 +107,42 @@
   </si>
   <si>
     <t>LRSR</t>
+  </si>
+  <si>
+    <t>max(lambda(t))</t>
+  </si>
+  <si>
+    <t>max(lambda(t)</t>
+  </si>
+  <si>
+    <t>proportional scale of control intensity</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>maximum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> control intensity over all simulations and over time</t>
+    </r>
+  </si>
+  <si>
+    <t>MCM</t>
+  </si>
+  <si>
+    <t>Qx = 1.0 / Qlam = _</t>
   </si>
 </sst>
 </file>
@@ -152,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -251,11 +288,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -283,6 +346,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,11 +663,397 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586D2981-F11D-FF41-B2CA-4D9EEFA82BCA}">
+  <dimension ref="B1:O21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="6.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="4.5" customWidth="1"/>
+    <col min="8" max="8" width="4.5" customWidth="1"/>
+    <col min="10" max="10" width="4.5" customWidth="1"/>
+    <col min="12" max="12" width="4.5" customWidth="1"/>
+    <col min="14" max="14" width="4.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" s="1" customFormat="1"/>
+    <row r="2" spans="2:15" s="1" customFormat="1">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="2:15" s="1" customFormat="1">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="2:15" s="1" customFormat="1">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" s="1" customFormat="1">
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" s="1" customFormat="1">
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" s="1" customFormat="1"/>
+    <row r="8" spans="2:15" s="1" customFormat="1"/>
+    <row r="9" spans="2:15" s="3" customFormat="1" ht="34">
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" s="1" customFormat="1">
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" s="1" customFormat="1">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="2:15" s="1" customFormat="1">
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1</v>
+      </c>
+      <c r="D12" s="10">
+        <v>163.30000000000001</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="H12" s="18"/>
+      <c r="I12" s="25">
+        <v>0.09</v>
+      </c>
+      <c r="K12" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="M12" s="25">
+        <v>5</v>
+      </c>
+      <c r="O12" s="25"/>
+    </row>
+    <row r="13" spans="2:15" s="1" customFormat="1">
+      <c r="B13" s="7">
+        <v>10</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="13">
+        <v>719.4</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="H13" s="18"/>
+      <c r="I13" s="26">
+        <v>0.06</v>
+      </c>
+      <c r="K13" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="M13" s="26">
+        <v>50</v>
+      </c>
+      <c r="O13" s="26"/>
+    </row>
+    <row r="14" spans="2:15" s="1" customFormat="1">
+      <c r="B14" s="7">
+        <v>20</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13">
+        <v>881.16669999999999</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="H14" s="18"/>
+      <c r="I14" s="26">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K14" s="26">
+        <v>0.06</v>
+      </c>
+      <c r="M14" s="26">
+        <v>90</v>
+      </c>
+      <c r="O14" s="26"/>
+    </row>
+    <row r="15" spans="2:15" s="1" customFormat="1">
+      <c r="B15" s="7">
+        <v>50</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="13">
+        <v>991.1</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="18"/>
+      <c r="I15" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="K15" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="M15" s="28">
+        <v>100</v>
+      </c>
+      <c r="O15" s="28"/>
+    </row>
+    <row r="16" spans="2:15" s="1" customFormat="1">
+      <c r="B16" s="7">
+        <v>100</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="13">
+        <v>911.03330000000005</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H16" s="18"/>
+      <c r="I16" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="K16" s="26">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M16" s="26">
+        <v>90</v>
+      </c>
+      <c r="O16" s="26"/>
+    </row>
+    <row r="17" spans="2:15" s="1" customFormat="1">
+      <c r="B17" s="7">
+        <v>150</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="13">
+        <v>732.8</v>
+      </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H17" s="18"/>
+      <c r="I17" s="26">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="K17" s="26">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="M17" s="26">
+        <v>50</v>
+      </c>
+      <c r="O17" s="26"/>
+    </row>
+    <row r="18" spans="2:15" s="1" customFormat="1">
+      <c r="B18" s="7">
+        <v>200</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+      <c r="D18" s="13">
+        <v>615.86670000000004</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="H18" s="18"/>
+      <c r="I18" s="26">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="K18" s="26">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="M18" s="26">
+        <v>40</v>
+      </c>
+      <c r="O18" s="26"/>
+    </row>
+    <row r="19" spans="2:15" s="1" customFormat="1">
+      <c r="B19" s="7">
+        <v>300</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="13">
+        <v>356.1</v>
+      </c>
+      <c r="E19" s="15">
+        <v>19.5352</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H19" s="18"/>
+      <c r="I19" s="26">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="K19" s="26">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="M19" s="26">
+        <v>22</v>
+      </c>
+      <c r="O19" s="26"/>
+    </row>
+    <row r="20" spans="2:15" s="1" customFormat="1">
+      <c r="B20" s="7">
+        <v>400</v>
+      </c>
+      <c r="C20" s="24">
+        <v>1</v>
+      </c>
+      <c r="D20" s="13">
+        <v>280.03309999999999</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="H20" s="18"/>
+      <c r="I20" s="26">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="K20" s="26">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M20" s="26">
+        <v>8</v>
+      </c>
+      <c r="O20" s="26"/>
+    </row>
+    <row r="21" spans="2:15" s="1" customFormat="1">
+      <c r="B21" s="7">
+        <v>500</v>
+      </c>
+      <c r="C21" s="19">
+        <v>1</v>
+      </c>
+      <c r="D21" s="20">
+        <v>166.66669999999999</v>
+      </c>
+      <c r="E21" s="22"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="19">
+        <v>7.6999999999999996E-4</v>
+      </c>
+      <c r="H21" s="18"/>
+      <c r="I21" s="27">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="K21" s="27">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="M21" s="27">
+        <v>6</v>
+      </c>
+      <c r="O21" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3BCD401-927F-E243-855F-63822595DF2B}">
-  <dimension ref="B2:Z33"/>
+  <dimension ref="B2:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Y18" sqref="Y18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1366,21 +1819,6 @@
       <c r="O25" s="17"/>
       <c r="P25" s="17"/>
     </row>
-    <row r="26" spans="2:26">
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>